<commit_message>
Update co2 supply curves numbers with latest from Daniel Wendt
</commit_message>
<xml_diff>
--- a/use_cases/2022_05/data/co2_supply_curves.xlsx
+++ b/use_cases/2022_05/data/co2_supply_curves.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garrm\projects\FORCE\use_cases\2022_05\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/projects/FORCE/use_cases/2022_05/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBA03AD-3FFD-42CF-805E-ABD04D1C9047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A372ADAA-0944-3542-9970-153A67585D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31020" yWindow="1290" windowWidth="16635" windowHeight="17190" activeTab="3" xr2:uid="{D53B6B06-4856-41C2-AFE8-9ACAA3E37143}"/>
+    <workbookView xWindow="7360" yWindow="1300" windowWidth="19460" windowHeight="21640" activeTab="3" xr2:uid="{D53B6B06-4856-41C2-AFE8-9ACAA3E37143}"/>
   </bookViews>
   <sheets>
     <sheet name="Braidwood" sheetId="1" r:id="rId1"/>
@@ -79,9 +79,6 @@
     <t>Cumulative Avg. Logistics cost of CO2 ($/MT)</t>
   </si>
   <si>
-    <t>co2 (kg/h)</t>
-  </si>
-  <si>
     <t>cost ($/kg)</t>
   </si>
   <si>
@@ -149,6 +146,9 @@
   </si>
   <si>
     <t>Craig</t>
+  </si>
+  <si>
+    <t>co2 (kg/year)</t>
   </si>
 </sst>
 </file>
@@ -502,19 +502,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B18B853-36C8-45C4-A6D0-11C71B7D9669}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F25"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -525,32 +525,32 @@
         <v>12</v>
       </c>
       <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.67700000000000005</v>
+        <v>0.68</v>
       </c>
       <c r="C2">
-        <v>12.1</v>
+        <v>11.95</v>
       </c>
       <c r="D2">
-        <f>B2*1000000000/(365*24)</f>
-        <v>77283.105022831049</v>
+        <f>B2*1000000</f>
+        <v>680000</v>
       </c>
       <c r="E2">
         <f>C2/1000</f>
-        <v>1.21E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.1949999999999999E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -558,56 +558,56 @@
         <v>1.37</v>
       </c>
       <c r="C3">
-        <v>15.56</v>
+        <v>15.39</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D11" si="0">B3*1000000000/(365*24)</f>
-        <v>156392.69406392693</v>
+        <f t="shared" ref="D3:D11" si="0">B3*1000000</f>
+        <v>1370000</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E11" si="1">C3/1000</f>
-        <v>1.5560000000000001E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.5390000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1.911</v>
+        <v>1.91</v>
       </c>
       <c r="C4">
-        <v>17.170000000000002</v>
+        <v>17</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>218150.68493150684</v>
+        <v>1910000</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>1.7170000000000001E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>2.1890000000000001</v>
+        <v>2.19</v>
       </c>
       <c r="C5">
-        <v>17.7</v>
+        <v>17.54</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>249885.84474885845</v>
+        <v>2190000</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>1.77E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.754E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -615,110 +615,110 @@
         <v>2.44</v>
       </c>
       <c r="C6">
-        <v>19.920000000000002</v>
+        <v>19.75</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>278538.81278538815</v>
+        <v>2440000</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>1.992E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.975E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>2.6909999999999998</v>
+        <v>2.69</v>
       </c>
       <c r="C7">
-        <v>22.29</v>
+        <v>22.11</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>307191.78082191781</v>
+        <v>2690000</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>2.2290000000000001E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.2109999999999998E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>2.859</v>
+        <v>2.86</v>
       </c>
       <c r="C8">
-        <v>23.7</v>
+        <v>23.53</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>326369.8630136986</v>
+        <v>2860000</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>2.3699999999999999E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.3530000000000002E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>3.0282</v>
+        <v>3.03</v>
       </c>
       <c r="C9">
-        <v>25.34</v>
+        <v>25.17</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>345684.9315068493</v>
+        <v>3030000</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>2.5340000000000001E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.5170000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>3.218</v>
+        <v>3.22</v>
       </c>
       <c r="C10">
-        <v>27.29</v>
+        <v>27.12</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>367351.59817351599</v>
+        <v>3220000</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>2.7289999999999998E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.7120000000000002E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>3.319</v>
+        <v>3.32</v>
       </c>
       <c r="C11">
-        <v>28.69</v>
+        <v>28.52</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>378881.27853881277</v>
+        <v>3320000</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>2.869E-2</v>
+        <v>2.852E-2</v>
       </c>
     </row>
   </sheetData>
@@ -730,18 +730,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE042658-68F7-4CD9-AA86-7BE66411A562}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="39.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -752,162 +752,162 @@
         <v>12</v>
       </c>
       <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>15</v>
       </c>
       <c r="B2">
         <v>0.24</v>
       </c>
       <c r="C2">
-        <v>23.6</v>
+        <v>23.49</v>
       </c>
       <c r="D2">
-        <f>B2*1000000000/(365*24)</f>
-        <v>27397.260273972603</v>
+        <f>B2*1000000</f>
+        <v>240000</v>
       </c>
       <c r="E2">
         <f>C2/1000</f>
-        <v>2.3600000000000003E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.3489999999999997E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>0.52</v>
       </c>
       <c r="C3">
-        <v>24.97</v>
+        <v>24.85</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D11" si="0">B3*1000000000/(365*24)</f>
-        <v>59360.730593607303</v>
+        <f t="shared" ref="D3:D9" si="0">B3*1000000</f>
+        <v>520000</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E11" si="1">C3/1000</f>
-        <v>2.4969999999999999E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <f t="shared" ref="E3:E9" si="1">C3/1000</f>
+        <v>2.4850000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>0.76</v>
       </c>
       <c r="C4">
-        <v>29.54</v>
+        <v>29.42</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>86757.990867579909</v>
+        <v>760000</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>2.954E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.9420000000000002E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>0.97</v>
       </c>
       <c r="C5">
-        <v>32.299999999999997</v>
+        <v>32.18</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>110730.59360730594</v>
+        <v>970000</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>3.2299999999999995E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>3.218E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>1.07</v>
       </c>
       <c r="C6">
-        <v>35.39</v>
+        <v>35.28</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>122146.1187214612</v>
+        <v>1070000</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>3.5389999999999998E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>3.5279999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7">
         <v>1.18</v>
       </c>
       <c r="C7">
-        <v>40.090000000000003</v>
+        <v>39.979999999999997</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>134703.19634703198</v>
+        <v>1180000</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>4.0090000000000001E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>3.9979999999999995E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8">
         <v>1.27</v>
       </c>
       <c r="C8">
-        <v>43.54</v>
+        <v>43.43</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>144977.1689497717</v>
+        <v>1270000</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>4.3540000000000002E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>4.3429999999999996E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9">
         <v>1.34</v>
       </c>
       <c r="C9">
-        <v>47.78</v>
+        <v>47.67</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>152968.03652968036</v>
+        <v>1340000</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>4.7780000000000003E-2</v>
+        <v>4.7670000000000004E-2</v>
       </c>
     </row>
   </sheetData>
@@ -919,20 +919,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28CF5BAD-BA4F-4815-A494-C3CAA4011C21}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -943,162 +943,162 @@
         <v>12</v>
       </c>
       <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>0.28000000000000003</v>
       </c>
       <c r="C2">
-        <v>28.52</v>
+        <v>28.34</v>
       </c>
       <c r="D2">
-        <f>B2*1000000000/(365*24)</f>
-        <v>31963.470319634704</v>
+        <f>B2*1000000</f>
+        <v>280000</v>
       </c>
       <c r="E2">
         <f>C2/1000</f>
-        <v>2.852E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.8340000000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>0.41</v>
       </c>
       <c r="C3">
-        <v>30.09</v>
+        <v>29.94</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D11" si="0">B3*1000000000/(365*24)</f>
-        <v>46803.652968036527</v>
+        <f t="shared" ref="D3:D9" si="0">B3*1000000</f>
+        <v>410000</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E11" si="1">C3/1000</f>
-        <v>3.0089999999999999E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <f t="shared" ref="E3:E9" si="1">C3/1000</f>
+        <v>2.9940000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <v>0.59</v>
       </c>
       <c r="C4">
-        <v>32.93</v>
+        <v>32.78</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>67351.598173515988</v>
+        <v>590000</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>3.2930000000000001E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>3.2780000000000004E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5">
         <v>0.84</v>
       </c>
       <c r="C5">
-        <v>39.57</v>
+        <v>39.39</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>95890.410958904104</v>
+        <v>840000</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>3.9570000000000001E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>3.9390000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6">
         <v>1.0900000000000001</v>
       </c>
       <c r="C6">
-        <v>44.1</v>
+        <v>43.9</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>124429.22374429223</v>
+        <v>1090000</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>4.41E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>4.3900000000000002E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <v>1.19</v>
       </c>
       <c r="C7">
-        <v>47.69</v>
+        <v>47.5</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>135844.74885844748</v>
+        <v>1190000</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>4.7689999999999996E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>4.7500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8">
         <v>1.3</v>
       </c>
       <c r="C8">
-        <v>53.5</v>
+        <v>53.32</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>148401.82648401827</v>
+        <v>1300000</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>5.3499999999999999E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>5.3319999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9">
         <v>1.39</v>
       </c>
       <c r="C9">
-        <v>58.62</v>
+        <v>58.44</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>158675.79908675799</v>
+        <v>1390000</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>5.8619999999999998E-2</v>
+        <v>5.8439999999999999E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1110,13 +1110,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00BF2B8C-0FE1-422D-BE97-FCE3E84E584D}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1127,124 +1127,124 @@
         <v>12</v>
       </c>
       <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>0.39</v>
       </c>
       <c r="C2">
-        <v>26.48</v>
+        <v>26.21</v>
       </c>
       <c r="D2">
-        <f>B2*1000000000/(365*24)</f>
-        <v>44520.547945205479</v>
+        <f>B2*1000000</f>
+        <v>390000</v>
       </c>
       <c r="E2">
         <f>C2/1000</f>
-        <v>2.648E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.6210000000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>0.56999999999999995</v>
       </c>
       <c r="C3">
-        <v>26.94</v>
+        <v>26.73</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D11" si="0">B3*1000000000/(365*24)</f>
-        <v>65068.493150684932</v>
+        <f t="shared" ref="D3:D7" si="0">B3*1000000</f>
+        <v>570000</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E11" si="1">C3/1000</f>
-        <v>2.6940000000000002E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <f t="shared" ref="E3:E7" si="1">C3/1000</f>
+        <v>2.673E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4">
         <v>0.76</v>
       </c>
       <c r="C4">
-        <v>28.92</v>
+        <v>28.74</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>86757.990867579909</v>
+        <v>760000</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>2.8920000000000001E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.8739999999999998E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5">
         <v>0.91</v>
       </c>
       <c r="C5">
-        <v>30.3</v>
+        <v>30.14</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>103881.27853881278</v>
+        <v>910000</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>3.0300000000000001E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>3.014E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
-        <v>34.85</v>
+        <v>34.69</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>114155.25114155251</v>
+        <v>1000000</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>3.4849999999999999E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>3.4689999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7">
         <v>1.04</v>
       </c>
       <c r="C7">
-        <v>38.18</v>
+        <v>38.03</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>118721.46118721461</v>
+        <v>1040000</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>3.8179999999999999E-2</v>
+        <v>3.8030000000000001E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>